<commit_message>
Question add feature, Question generation modification, added SE or EE type question in Question generation
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24703"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssss\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE0609B-359E-486F-A144-4EAF35A690C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC9C690D-7ED2-4ECE-862F-52B03A5596FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{9FB0A0DE-274F-4FAD-A09C-E1958604F425}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>body</t>
   </si>
@@ -39,6 +48,9 @@
     <t>Why is Java a platform independent language?</t>
   </si>
   <si>
+    <t>SE</t>
+  </si>
+  <si>
     <t>What is an Optional class?</t>
   </si>
   <si>
@@ -81,14 +93,59 @@
     <t>Java Medium Question $$$$$$$$$$$</t>
   </si>
   <si>
-    <t>SE</t>
+    <t>the final variable is used to restrict the user from updating it. If we initialize the final variable, we can't change its value</t>
+  </si>
+  <si>
+    <t>Compiletime Error because of final variable can't be update</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Compiletime error. Because final method can't be override</t>
+  </si>
+  <si>
+    <t>The interface is a blueprint for a class that has static constants and abstract methods. It can be used to achieve full abstraction and multiple inheritance. It is a mechanism to achieve abstraction. There can be only abstract methods in the Java interface, not method body. It is used to achieve abstraction and multiple inheritance in Java.</t>
+  </si>
+  <si>
+    <t>Exception Handling is a mechanism that is used to handle runtime errors</t>
+  </si>
+  <si>
+    <t>a equals b</t>
+  </si>
+  <si>
+    <t>Garbage collection is a process of reclaiming the unused runtime objects. It is performed for memory management.</t>
+  </si>
+  <si>
+    <t>Serialization in Java is a mechanism of writing the state of an object into a byte stream. It is used primarily in Hibernate, RMI, JPA, EJB and JMS technologies.</t>
+  </si>
+  <si>
+    <t>Java Socket programming is used for communication between the applications running on different JRE. Java Socket programming can be connection-oriented or connectionless. Socket and ServerSocket classes are used for connection-oriented socket programming and DatagramSocket, and DatagramPacket classes are used for connectionless socket programming.</t>
+  </si>
+  <si>
+    <t>A socket is simply an endpoint for communications between the machines. It provides the connection mechanism to connect the two computers using TCP. The Socket class can be used to create a socket.</t>
+  </si>
+  <si>
+    <t>Reflection is the process of examining or modifying the runtime behavior of a class at runtime. The java.lang.Class class provides various methods that can be used to get metadata, examine and change the runtime behavior of a class.</t>
+  </si>
+  <si>
+    <t>What is the purpose of wait() method in Java?</t>
+  </si>
+  <si>
+    <t>What are the states in the lifecycle of a Thread?</t>
+  </si>
+  <si>
+    <t>What does join() method?</t>
+  </si>
+  <si>
+    <t>What is the deadlock?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +161,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -121,13 +184,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,18 +559,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0EB5BB-F45E-4A76-B100-432EBE7796B3}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="93.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,169 +581,334 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="25.5">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="51">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="25.5">
+      <c r="A23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="25.5">
+      <c r="A24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="51">
+      <c r="A25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="25.5">
+      <c r="A26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="38.25">
+      <c r="A27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>